<commit_message>
memperbaiki no. 4 dan menambahkan no. yang belum
</commit_message>
<xml_diff>
--- a/SyarifYahya/data.xlsx
+++ b/SyarifYahya/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,16 @@
           <t>Nilai Akhir</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Rank</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Rata Rata</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -478,6 +488,12 @@
       <c r="E2" t="n">
         <v>81</v>
       </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -497,6 +513,12 @@
       <c r="E3" t="n">
         <v>79</v>
       </c>
+      <c r="F3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -516,6 +538,12 @@
       <c r="E4" t="n">
         <v>80</v>
       </c>
+      <c r="F4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -535,6 +563,12 @@
       <c r="E5" t="n">
         <v>78</v>
       </c>
+      <c r="F5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G5" t="n">
+        <v>76.7</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -554,6 +588,12 @@
       <c r="E6" t="n">
         <v>68</v>
       </c>
+      <c r="F6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" t="n">
+        <v>66.7</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -573,6 +613,12 @@
       <c r="E7" t="n">
         <v>58</v>
       </c>
+      <c r="F7" t="n">
+        <v>11</v>
+      </c>
+      <c r="G7" t="n">
+        <v>56.7</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -592,6 +638,12 @@
       <c r="E8" t="n">
         <v>48</v>
       </c>
+      <c r="F8" t="n">
+        <v>12</v>
+      </c>
+      <c r="G8" t="n">
+        <v>46.7</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -611,6 +663,12 @@
       <c r="E9" t="n">
         <v>38</v>
       </c>
+      <c r="F9" t="n">
+        <v>13</v>
+      </c>
+      <c r="G9" t="n">
+        <v>36.7</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -630,6 +688,12 @@
       <c r="E10" t="n">
         <v>28</v>
       </c>
+      <c r="F10" t="n">
+        <v>14</v>
+      </c>
+      <c r="G10" t="n">
+        <v>26.7</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -649,6 +713,12 @@
       <c r="E11" t="n">
         <v>18</v>
       </c>
+      <c r="F11" t="n">
+        <v>15</v>
+      </c>
+      <c r="G11" t="n">
+        <v>16.7</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -668,6 +738,12 @@
       <c r="E12" t="n">
         <v>74.40000000000001</v>
       </c>
+      <c r="F12" t="n">
+        <v>9</v>
+      </c>
+      <c r="G12" t="n">
+        <v>76</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -687,6 +763,12 @@
       <c r="E13" t="n">
         <v>81</v>
       </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -706,6 +788,12 @@
       <c r="E14" t="n">
         <v>79</v>
       </c>
+      <c r="F14" t="n">
+        <v>5</v>
+      </c>
+      <c r="G14" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -725,6 +813,12 @@
       <c r="E15" t="n">
         <v>80</v>
       </c>
+      <c r="F15" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -743,6 +837,12 @@
       </c>
       <c r="E16" t="n">
         <v>78</v>
+      </c>
+      <c r="F16" t="n">
+        <v>7</v>
+      </c>
+      <c r="G16" t="n">
+        <v>76.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>